<commit_message>
Update: Fixed the merged repo issues in Helios300. Fixed the live trading backfill in BT by taking the latest commit from the ftomassetti/backtrader-oandav20
</commit_message>
<xml_diff>
--- a/Storage/airflow/dags/interested_tickers.xlsx
+++ b/Storage/airflow/dags/interested_tickers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google drive\Business\Repos\QuantInfra\airflow\dags\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google drive\Business\Repos\Quant-Trading-Infrastructure\Storage\airflow\dags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E770837-0C37-401C-B12A-E822FFD085A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A116D94E-F504-43FE-A0EA-88564AE73BAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57120" yWindow="660" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-55680" yWindow="2100" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Tickers</t>
   </si>
@@ -358,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -381,6 +381,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -390,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833803CE-59C3-4CA2-B52B-89F040AAE3D2}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>